<commit_message>
CARGA ARCHIVO Campo El pichi, doble cultivo, doble siembra por cultivo
</commit_message>
<xml_diff>
--- a/carga/PLAN SIEMBRA  EL PICHI 22-23 (2) (1).xlsx
+++ b/carga/PLAN SIEMBRA  EL PICHI 22-23 (2) (1).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5364C1E5-0B93-417C-AB2D-AC3BE886809B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B0C750-9CA4-4008-ACBC-7E72CE695EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="2460" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -294,9 +294,6 @@
     <t>70 HAS VICIA TRITICALE COBERTURA RESTO LOTE MAIZ PRIMERA</t>
   </si>
   <si>
-    <t>VICIA TRITICALE/MAIZ 2DA MAIZ 1ERA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trigo </t>
   </si>
   <si>
@@ -331,6 +328,9 @@
   </si>
   <si>
     <t>340 u$s/ha</t>
+  </si>
+  <si>
+    <t>VICIA-TRITICALE/MAIZ 2DA-MAIZ 1ERA</t>
   </si>
 </sst>
 </file>
@@ -949,7 +949,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H6"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +958,7 @@
     <col min="2" max="2" width="7.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="29.5703125" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" customWidth="1"/>
+    <col min="5" max="5" width="59.5703125" customWidth="1"/>
     <col min="6" max="6" width="42.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -972,10 +972,10 @@
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="G1" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="39" t="s">
         <v>90</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.25">
@@ -983,18 +983,18 @@
         <v>65</v>
       </c>
       <c r="G2" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="39" t="s">
         <v>92</v>
-      </c>
-      <c r="H2" s="39" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G3" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="39" t="s">
         <v>94</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1002,10 +1002,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="39" t="s">
         <v>96</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
@@ -1013,10 +1013,10 @@
         <v>64</v>
       </c>
       <c r="G5" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="39" t="s">
         <v>98</v>
-      </c>
-      <c r="H5" s="39" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1027,10 +1027,10 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="39" t="s">
         <v>100</v>
-      </c>
-      <c r="H6" s="39" t="s">
-        <v>101</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -1247,7 +1247,7 @@
         <v>88</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="3"/>

</xml_diff>

<commit_message>
Carga Archivo Planificacion -conf Campo el Pichi
</commit_message>
<xml_diff>
--- a/carga/PLAN SIEMBRA  EL PICHI 22-23 (2) (1).xlsx
+++ b/carga/PLAN SIEMBRA  EL PICHI 22-23 (2) (1).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B0C750-9CA4-4008-ACBC-7E72CE695EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409B4E63-4B4D-4C2A-8727-8A47D3DB6601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2460" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilla" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="102">
   <si>
     <t>Plan de siembra</t>
   </si>
@@ -330,7 +330,7 @@
     <t>340 u$s/ha</t>
   </si>
   <si>
-    <t>VICIA-TRITICALE/MAIZ 2DA-MAIZ 1ERA</t>
+    <t>VICIA-TRITICALE/MAIZ 2DA</t>
   </si>
 </sst>
 </file>
@@ -949,7 +949,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1235,7 @@
         <v>54</v>
       </c>
       <c r="B15" s="2">
-        <v>138</v>
+        <v>70</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>63</v>
@@ -1260,22 +1260,22 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="B16" s="2">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="G16" s="23"/>
       <c r="H16" s="3"/>
@@ -1288,22 +1288,22 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="G17" s="23"/>
       <c r="H17" s="3"/>
@@ -1316,19 +1316,23 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="4">
-        <v>42</v>
+        <v>48</v>
+      </c>
+      <c r="B18" s="2">
+        <v>89</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="G18" s="23"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1340,10 +1344,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="4">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>9</v>
@@ -1364,10 +1368,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="4">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
@@ -1386,10 +1390,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="4">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>9</v>
@@ -1408,10 +1412,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="4">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>9</v>
@@ -1429,20 +1433,29 @@
       <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="6">
-        <f>SUM(B8:B22)</f>
-        <v>732</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="6">
+        <f>SUM(B9:B23)</f>
+        <v>703</v>
+      </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>

</xml_diff>